<commit_message>
Database Schema and UI updated. Fertilizer Recommendations updated. Slight UI Modifications.
</commit_message>
<xml_diff>
--- a/Test Reports/2656_test.xlsx
+++ b/Test Reports/2656_test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,6 +522,11 @@
           <t>Recommendations</t>
         </is>
       </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Fertilizer Recommendation</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -535,67 +540,72 @@
         </is>
       </c>
       <c r="C2" t="n">
+        <v>656</v>
+      </c>
+      <c r="D2" t="n">
+        <v>656</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>asdasdasd</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>52</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>65</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>23323as2d3asd</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>6556456464</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
         <v>232</v>
-      </c>
-      <c r="D2" t="n">
-        <v>232</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>asdlaksdlasd</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>26</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>23</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>565656as2d32asd</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>9898656232</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>5</v>
-      </c>
-      <c r="L2" t="n">
-        <v>23</v>
       </c>
       <c r="M2" t="n">
         <v>32</v>
       </c>
       <c r="N2" t="n">
-        <v>256</v>
+        <v>200</v>
       </c>
       <c r="O2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P2" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="Q2" t="n">
         <v>32</v>
       </c>
       <c r="R2" t="n">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="S2" t="n">
-        <v>0.3404714934752574</v>
+        <v>0.331370118203286</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
           <t>Grow millets (sorghum, pearl millet), pulses (pigeon pea, chickpea), and oilseeds (safflower, castor).</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>No specific fertilizer recommendation available for the given soil data.</t>
         </is>
       </c>
     </row>

</xml_diff>